<commit_message>
Update 2020182051전태준 졸업작품 계획표.xlsx
</commit_message>
<xml_diff>
--- a/졸업작품 제안서/2020182051전태준 졸업작품 계획표.xlsx
+++ b/졸업작품 제안서/2020182051전태준 졸업작품 계획표.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <x:si>
     <x:t>엔진 내부 구조에 친숙해지기 핵심 5개 클래스(UObject
 Actor
@@ -28,151 +28,142 @@
 Character)</x:t>
   </x:si>
   <x:si>
-    <x:t>복습</x:t>
-  </x:si>
-  <x:si>
-    <x:t>직렬화</x:t>
+    <x:t>엔진 초기화 소스코드 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>퍼시스턴트레벨 로딩 코드분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>시간 날때 블렌더 공부하기</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(엔진 오브젝트 리플렉션)</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> </x:t>
+  </x:si>
+  <x:si>
+    <x:t>??</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7월 3주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(인터페이스)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9월 1주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11월 4주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6월 4주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8월 1주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2학기중 계획</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7월 2주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(델리게이트)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(컴포지션)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9월 2주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10월 3주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10월 4주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>중간고사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12월 1주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9월 4주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9월 3주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11월 3주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">상호작용 </x:t>
+  </x:si>
+  <x:si>
+    <x:t>8월 2주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11월 1주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8월 3주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7월 1주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10월 2주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>기말고사</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8월 4주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7월 4주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10월 1주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11월 2주차</x:t>
+  </x:si>
+  <x:si>
+    <x:t>언리얼엔진 Lanch 소스코드 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ai 시스템 구현</x:t>
+  </x:si>
+  <x:si>
+    <x:t>로코모션,공격 구현</x:t>
+  </x:si>
+  <x:si>
+    <x:t>방학 기간 계획</x:t>
+  </x:si>
+  <x:si>
+    <x:t>component제작</x:t>
+  </x:si>
+  <x:si>
+    <x:t>언리얼 엔진 c++</x:t>
   </x:si>
   <x:si>
     <x:t>적 오브젝트 component 제작</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">A* 길찾기 알고리즘으로 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>(엔진 오브젝트 리플렉션)</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">캐릭터 애니메이션/공격 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>시간 날때 블렌더 공부하기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>언리얼 컨테이너 라이브러리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>캐릭터 입력/컨트롤 설정</x:t>
-  </x:si>
-  <x:si>
-    <x:t>패키지,에셋</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7월 3주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9월 2주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2학기중 계획</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9월 1주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ㄴ렌더링파트</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6월 4주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>중간고사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(컴포지션)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(인터페이스)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11월 4주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10월 3주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(델리게이트)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10월 4주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7월 2주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12월 1주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9월 4주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9월 3주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8월 1주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8월 4주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11월 1주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>기말고사</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11월 2주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8월 3주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11월 3주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10월 2주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8월 2주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7월 4주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7월 1주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10월 1주차</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">상호작용 </x:t>
+    <x:t>procedural mesh(동적 메쉬 절단) 제작…</x:t>
   </x:si>
   <x:si>
     <x:t>간단한 토이프로젝트 제작하면서 필요한 부분 찾아보고</x:t>
   </x:si>
   <x:si>
-    <x:t>procedural mesh(동적 메쉬 절단) 제작…</x:t>
-  </x:si>
-  <x:si>
-    <x:t>언리얼 엔진 내부구조</x:t>
-  </x:si>
-  <x:si>
-    <x:t>방학 기간 계획</x:t>
-  </x:si>
-  <x:si>
-    <x:t>언리얼엔진 내부구조</x:t>
-  </x:si>
-  <x:si>
-    <x:t>component제작</x:t>
-  </x:si>
-  <x:si>
-    <x:t>언리얼엔진 c++</x:t>
-  </x:si>
-  <x:si>
-    <x:t>언리얼 엔진 c++</x:t>
-  </x:si>
-  <x:si>
-    <x:t>목표 까지 길찾아주는 component 제작</x:t>
+    <x:t>월드생성 코드 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>입력시스템 다시 ue5 버전으로구현,</x:t>
   </x:si>
   <x:si>
     <x:t>Main캐릭터관련 component 제작</x:t>
@@ -845,7 +836,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="63">
+  <x:cellXfs count="65">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -1501,6 +1492,32 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -2197,22 +2214,22 @@
   <x:sheetPr codeName="Sheet1"/>
   <x:dimension ref="A9:S39"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="I3" activeCellId="0" sqref="I3:I3"/>
+    <x:sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <x:selection activeCell="M8" activeCellId="0" sqref="M8:M8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="16.399999999999999"/>
   <x:cols>
     <x:col min="3" max="3" width="18.19921875" style="1" customWidth="1"/>
     <x:col min="5" max="5" width="20.796875" style="1" customWidth="1"/>
-    <x:col min="7" max="7" width="17.59765625" style="1" customWidth="1"/>
+    <x:col min="7" max="7" width="25.6015625" style="1" customWidth="1"/>
     <x:col min="9" max="9" width="12.5" style="1" customWidth="1"/>
-    <x:col min="11" max="11" width="12.5" style="1" customWidth="1"/>
+    <x:col min="11" max="11" width="23.6015625" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="9" spans="2:19">
       <x:c r="B9" s="37" t="s">
-        <x:v>44</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C9" s="38"/>
       <x:c r="D9" s="38"/>
@@ -2255,65 +2272,65 @@
     </x:row>
     <x:row r="11" spans="2:19" ht="16.75">
       <x:c r="B11" s="47" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C11" s="48"/>
       <x:c r="D11" s="49" t="s">
-        <x:v>38</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E11" s="48"/>
       <x:c r="F11" s="43" t="s">
-        <x:v>24</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G11" s="50"/>
       <x:c r="H11" s="43" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="I11" s="50"/>
       <x:c r="J11" s="43" t="s">
-        <x:v>37</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="K11" s="50"/>
       <x:c r="L11" s="43" t="s">
-        <x:v>28</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="M11" s="50"/>
       <x:c r="N11" s="43" t="s">
-        <x:v>36</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="O11" s="44"/>
       <x:c r="P11" s="45" t="s">
-        <x:v>33</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="Q11" s="44"/>
       <x:c r="R11" s="43" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="S11" s="46"/>
     </x:row>
     <x:row r="12" spans="2:19">
       <x:c r="B12" s="51" t="s">
-        <x:v>48</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C12" s="52"/>
       <x:c r="D12" s="51" t="s">
-        <x:v>47</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E12" s="52"/>
-      <x:c r="F12" s="51" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="G12" s="52"/>
+      <x:c r="F12" s="63" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="G12" s="64"/>
       <x:c r="H12" s="51" t="s">
-        <x:v>43</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="I12" s="52"/>
       <x:c r="J12" s="51" t="s">
-        <x:v>43</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="K12" s="52"/>
       <x:c r="L12" s="51" t="s">
-        <x:v>41</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="M12" s="26"/>
       <x:c r="N12" s="26"/>
@@ -2328,8 +2345,8 @@
       <x:c r="C13" s="36"/>
       <x:c r="D13" s="35"/>
       <x:c r="E13" s="36"/>
-      <x:c r="F13" s="35"/>
-      <x:c r="G13" s="36"/>
+      <x:c r="F13" s="61"/>
+      <x:c r="G13" s="62"/>
       <x:c r="H13" s="35"/>
       <x:c r="I13" s="36"/>
       <x:c r="J13" s="35"/>
@@ -2345,21 +2362,21 @@
     </x:row>
     <x:row r="14" spans="2:19">
       <x:c r="B14" s="35" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C14" s="36"/>
       <x:c r="D14" s="35" t="s">
-        <x:v>8</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E14" s="36"/>
-      <x:c r="F14" s="35" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="G14" s="36"/>
-      <x:c r="H14" s="35"/>
+      <x:c r="F14" s="61"/>
+      <x:c r="G14" s="62"/>
+      <x:c r="H14" s="35" t="s">
+        <x:v>45</x:v>
+      </x:c>
       <x:c r="I14" s="36"/>
       <x:c r="J14" s="35" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="K14" s="36"/>
       <x:c r="L14" s="35"/>
@@ -2373,15 +2390,13 @@
     </x:row>
     <x:row r="15" spans="2:19">
       <x:c r="B15" s="61" t="s">
-        <x:v>19</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C15" s="62"/>
-      <x:c r="D15" s="35" t="s">
-        <x:v>2</x:v>
-      </x:c>
+      <x:c r="D15" s="35"/>
       <x:c r="E15" s="36"/>
-      <x:c r="F15" s="35"/>
-      <x:c r="G15" s="36"/>
+      <x:c r="F15" s="61"/>
+      <x:c r="G15" s="62"/>
       <x:c r="H15" s="35"/>
       <x:c r="I15" s="36"/>
       <x:c r="J15" s="35"/>
@@ -2399,15 +2414,13 @@
     </x:row>
     <x:row r="16" spans="2:19">
       <x:c r="B16" s="61" t="s">
-        <x:v>18</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C16" s="62"/>
-      <x:c r="D16" s="35" t="s">
-        <x:v>10</x:v>
-      </x:c>
+      <x:c r="D16" s="35"/>
       <x:c r="E16" s="36"/>
       <x:c r="F16" s="61" t="s">
-        <x:v>9</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="G16" s="62"/>
       <x:c r="H16" s="35"/>
@@ -2425,13 +2438,13 @@
     </x:row>
     <x:row r="17" spans="2:19">
       <x:c r="B17" s="61" t="s">
-        <x:v>22</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C17" s="62"/>
       <x:c r="D17" s="3"/>
       <x:c r="E17" s="4"/>
       <x:c r="F17" s="61" t="s">
-        <x:v>6</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G17" s="62"/>
       <x:c r="H17" s="3"/>
@@ -2509,7 +2522,7 @@
     </x:row>
     <x:row r="21" spans="2:19">
       <x:c r="B21" s="58" t="s">
-        <x:v>7</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="C21" s="59"/>
       <x:c r="D21" s="59"/>
@@ -2609,41 +2622,41 @@
     </x:row>
     <x:row r="28" spans="2:17" ht="16.75">
       <x:c r="B28" s="25" t="s">
-        <x:v>14</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C28" s="29"/>
       <x:c r="D28" s="25" t="s">
-        <x:v>12</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E28" s="29"/>
       <x:c r="F28" s="25" t="s">
-        <x:v>27</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G28" s="29"/>
       <x:c r="H28" s="25" t="s">
-        <x:v>26</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="I28" s="29"/>
       <x:c r="J28" s="25" t="s">
-        <x:v>39</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="K28" s="29"/>
       <x:c r="L28" s="25" t="s">
-        <x:v>35</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="M28" s="29"/>
       <x:c r="N28" s="25" t="s">
-        <x:v>21</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="O28" s="29"/>
       <x:c r="P28" s="25" t="s">
-        <x:v>23</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="Q28" s="29"/>
     </x:row>
     <x:row r="29" spans="2:17">
       <x:c r="B29" s="16" t="s">
-        <x:v>50</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C29" s="17"/>
       <x:c r="D29" s="17"/>
@@ -2651,7 +2664,7 @@
       <x:c r="F29" s="17"/>
       <x:c r="G29" s="17"/>
       <x:c r="H29" s="16" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="I29" s="17"/>
       <x:c r="J29" s="17"/>
@@ -2659,11 +2672,11 @@
       <x:c r="L29" s="17"/>
       <x:c r="M29" s="18"/>
       <x:c r="N29" s="16" t="s">
-        <x:v>17</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="O29" s="17"/>
       <x:c r="P29" s="16" t="s">
-        <x:v>40</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="Q29" s="18"/>
     </x:row>
@@ -2692,9 +2705,7 @@
       <x:c r="E31" s="8"/>
       <x:c r="F31" s="8"/>
       <x:c r="G31" s="8"/>
-      <x:c r="H31" s="22" t="s">
-        <x:v>49</x:v>
-      </x:c>
+      <x:c r="H31" s="22"/>
       <x:c r="I31" s="23"/>
       <x:c r="J31" s="23"/>
       <x:c r="K31" s="23"/>
@@ -2703,7 +2714,7 @@
       <x:c r="N31" s="14"/>
       <x:c r="O31" s="12"/>
       <x:c r="P31" s="19" t="s">
-        <x:v>46</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="Q31" s="21"/>
     </x:row>
@@ -2781,23 +2792,23 @@
     </x:row>
     <x:row r="36" spans="2:13" ht="17.149999999999999">
       <x:c r="B36" s="25" t="s">
-        <x:v>30</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C36" s="26"/>
       <x:c r="D36" s="26" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E36" s="26"/>
       <x:c r="F36" s="26" t="s">
-        <x:v>34</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="G36" s="26"/>
       <x:c r="H36" s="26" t="s">
-        <x:v>20</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="I36" s="26"/>
       <x:c r="J36" s="27" t="s">
-        <x:v>25</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="K36" s="27"/>
       <x:c r="L36" s="28"/>
@@ -2805,13 +2816,13 @@
     </x:row>
     <x:row r="37" spans="2:13">
       <x:c r="B37" s="16" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C37" s="17"/>
       <x:c r="D37" s="17"/>
       <x:c r="E37" s="18"/>
       <x:c r="F37" s="16" t="s">
-        <x:v>3</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="G37" s="17"/>
       <x:c r="H37" s="17"/>
@@ -2848,7 +2859,7 @@
       <x:c r="I39" s="24"/>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="55">
+  <x:mergeCells count="54">
     <x:mergeCell ref="B37:E39"/>
     <x:mergeCell ref="F37:I39"/>
     <x:mergeCell ref="J37:K38"/>
@@ -2892,8 +2903,6 @@
     <x:mergeCell ref="B21:K23"/>
     <x:mergeCell ref="D15:E15"/>
     <x:mergeCell ref="D16:E16"/>
-    <x:mergeCell ref="F12:G13"/>
-    <x:mergeCell ref="F14:G15"/>
     <x:mergeCell ref="B12:C13"/>
     <x:mergeCell ref="B14:C14"/>
     <x:mergeCell ref="D12:E13"/>
@@ -2904,8 +2913,9 @@
     <x:mergeCell ref="B17:C17"/>
     <x:mergeCell ref="F16:G16"/>
     <x:mergeCell ref="F17:G17"/>
+    <x:mergeCell ref="F12:G15"/>
   </x:mergeCells>
-  <x:pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <x:pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>